<commit_message>
fit : data importation
</commit_message>
<xml_diff>
--- a/backEnd/src/main/resources/dataFilieres.xlsx
+++ b/backEnd/src/main/resources/dataFilieres.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamid\Documents\GitHub\ProjetInnovation\PI_GESTION_EMPLOIS_TEMPS\backEnd\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PI_GESTION_EMPLOIS_TEMPS\backend\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC819E1-0638-4F6B-9F79-9FEE21194026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648F50FE-501A-42AB-9155-FEDC9A42E816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{5E0B78FC-6F57-4D7D-B7B9-2CAC3030FF9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{5E0B78FC-6F57-4D7D-B7B9-2CAC3030FF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="ENSEIGNANTS" sheetId="4" r:id="rId1"/>
@@ -919,14 +919,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
@@ -954,7 +954,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1252,11 +1252,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9931D10E-5844-45F1-BBD8-9F9833CB5A2C}">
   <dimension ref="C4:C73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="36.85546875" customWidth="1"/>
   </cols>
@@ -1624,11 +1624,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{779942B0-0B7F-4556-8888-7ED49D3C1B25}">
   <dimension ref="C4:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+    <sheetView topLeftCell="B13" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="36.85546875" customWidth="1"/>
     <col min="4" max="4" width="33.140625" customWidth="1"/>
@@ -1942,11 +1942,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9440788B-F075-4906-AEF1-F1D379CBA878}">
   <dimension ref="B1:G87"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2018,13 +2018,13 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -2038,9 +2038,9 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="2" t="s">
         <v>135</v>
       </c>
@@ -2052,11 +2052,11 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>59</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -2070,9 +2070,9 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="2" t="s">
         <v>136</v>
       </c>
@@ -2084,11 +2084,11 @@
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -2102,9 +2102,9 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="2" t="s">
         <v>137</v>
       </c>
@@ -2116,11 +2116,11 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -2134,9 +2134,9 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="2" t="s">
         <v>139</v>
       </c>
@@ -2148,11 +2148,11 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -2166,9 +2166,9 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="2" t="s">
         <v>141</v>
       </c>
@@ -2180,11 +2180,11 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -2198,9 +2198,9 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="2" t="s">
         <v>143</v>
       </c>
@@ -2212,11 +2212,11 @@
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -2230,9 +2230,9 @@
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="2" t="s">
         <v>145</v>
       </c>
@@ -2244,45 +2244,45 @@
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="G23" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
@@ -2294,11 +2294,11 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -2312,9 +2312,9 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="2" t="s">
         <v>147</v>
       </c>
@@ -2326,11 +2326,11 @@
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -2344,9 +2344,9 @@
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="2" t="s">
         <v>149</v>
       </c>
@@ -2358,11 +2358,11 @@
       </c>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -2376,9 +2376,9 @@
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="2" t="s">
         <v>151</v>
       </c>
@@ -2390,11 +2390,11 @@
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -2408,9 +2408,9 @@
       </c>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="13"/>
       <c r="E32" s="2" t="s">
         <v>153</v>
       </c>
@@ -2422,11 +2422,11 @@
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="12"/>
-      <c r="C33" s="12" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -2440,9 +2440,9 @@
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="2" t="s">
         <v>155</v>
       </c>
@@ -2454,11 +2454,11 @@
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="12"/>
-      <c r="C35" s="12" t="s">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -2472,9 +2472,9 @@
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="2" t="s">
         <v>157</v>
       </c>
@@ -2486,11 +2486,11 @@
       </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="12"/>
-      <c r="C37" s="12" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>82</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -2504,21 +2504,21 @@
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="13"/>
       <c r="E38" s="8"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -2532,9 +2532,9 @@
       </c>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="13"/>
       <c r="E40" s="2" t="s">
         <v>159</v>
       </c>
@@ -2546,11 +2546,11 @@
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="12"/>
-      <c r="C41" s="12" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -2564,9 +2564,9 @@
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="13"/>
       <c r="E42" s="2" t="s">
         <v>15</v>
       </c>
@@ -2578,11 +2578,11 @@
       </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="12"/>
-      <c r="C43" s="12" t="s">
+      <c r="B43" s="14"/>
+      <c r="C43" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -2596,9 +2596,9 @@
       </c>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="13"/>
       <c r="E44" s="2" t="s">
         <v>162</v>
       </c>
@@ -2610,11 +2610,11 @@
       </c>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="12"/>
-      <c r="C45" s="12" t="s">
+      <c r="B45" s="14"/>
+      <c r="C45" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>80</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -2628,9 +2628,9 @@
       </c>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="13"/>
       <c r="E46" s="2" t="s">
         <v>16</v>
       </c>
@@ -2642,11 +2642,11 @@
       </c>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="12"/>
-      <c r="C47" s="12" t="s">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -2660,9 +2660,9 @@
       </c>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="13"/>
       <c r="E48" s="2" t="s">
         <v>165</v>
       </c>
@@ -2674,11 +2674,11 @@
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="12"/>
-      <c r="C49" s="12" t="s">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -2692,9 +2692,9 @@
       </c>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="13"/>
       <c r="E50" s="2" t="s">
         <v>167</v>
       </c>
@@ -2706,11 +2706,11 @@
       </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="12"/>
-      <c r="C51" s="12" t="s">
+      <c r="B51" s="14"/>
+      <c r="C51" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -2724,9 +2724,9 @@
       </c>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="2" t="s">
         <v>169</v>
       </c>
@@ -2738,11 +2738,11 @@
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="12"/>
-      <c r="C53" s="12" t="s">
+      <c r="B53" s="14"/>
+      <c r="C53" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="12" t="s">
         <v>38</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -2754,21 +2754,21 @@
       </c>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="13"/>
       <c r="E54" s="8"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -2782,9 +2782,9 @@
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="2" t="s">
         <v>170</v>
       </c>
@@ -2796,11 +2796,11 @@
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="12"/>
-      <c r="C57" s="12" t="s">
+      <c r="B57" s="14"/>
+      <c r="C57" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -2814,9 +2814,9 @@
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="13"/>
       <c r="E58" s="2" t="s">
         <v>172</v>
       </c>
@@ -2828,11 +2828,11 @@
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="12"/>
-      <c r="C59" s="12" t="s">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -2846,9 +2846,9 @@
       </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="13"/>
       <c r="E60" s="2" t="s">
         <v>174</v>
       </c>
@@ -2860,11 +2860,11 @@
       </c>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="12"/>
-      <c r="C61" s="12" t="s">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -2878,9 +2878,9 @@
       </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="13"/>
       <c r="E62" s="2" t="s">
         <v>176</v>
       </c>
@@ -2892,11 +2892,11 @@
       </c>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="12"/>
-      <c r="C63" s="12" t="s">
+      <c r="B63" s="14"/>
+      <c r="C63" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E63" s="2" t="s">
@@ -2910,9 +2910,9 @@
       </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="13"/>
       <c r="E64" s="2" t="s">
         <v>177</v>
       </c>
@@ -2924,11 +2924,11 @@
       </c>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="12"/>
-      <c r="C65" s="12" t="s">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D65" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E65" s="2" t="s">
@@ -2942,9 +2942,9 @@
       </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="13"/>
       <c r="E66" s="2" t="s">
         <v>179</v>
       </c>
@@ -2956,11 +2956,11 @@
       </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="12"/>
-      <c r="C67" s="12" t="s">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -2974,9 +2974,9 @@
       </c>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="13"/>
       <c r="E68" s="2" t="s">
         <v>181</v>
       </c>
@@ -2988,11 +2988,11 @@
       </c>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="12"/>
-      <c r="C69" s="12" t="s">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E69" s="2" t="s">
@@ -3006,21 +3006,21 @@
       </c>
     </row>
     <row r="70" spans="2:7">
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="13"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:7">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -3034,9 +3034,9 @@
       </c>
     </row>
     <row r="72" spans="2:7">
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="13"/>
       <c r="E72" s="2" t="s">
         <v>184</v>
       </c>
@@ -3048,11 +3048,11 @@
       </c>
     </row>
     <row r="73" spans="2:7">
-      <c r="B73" s="12"/>
-      <c r="C73" s="12" t="s">
+      <c r="B73" s="14"/>
+      <c r="C73" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D73" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E73" s="2" t="s">
@@ -3066,9 +3066,9 @@
       </c>
     </row>
     <row r="74" spans="2:7">
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="13"/>
       <c r="E74" s="2" t="s">
         <v>186</v>
       </c>
@@ -3080,11 +3080,11 @@
       </c>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="12"/>
-      <c r="C75" s="12" t="s">
+      <c r="B75" s="14"/>
+      <c r="C75" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E75" s="2" t="s">
@@ -3098,9 +3098,9 @@
       </c>
     </row>
     <row r="76" spans="2:7">
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="13"/>
       <c r="E76" s="2" t="s">
         <v>188</v>
       </c>
@@ -3112,11 +3112,11 @@
       </c>
     </row>
     <row r="77" spans="2:7">
-      <c r="B77" s="12"/>
-      <c r="C77" s="12" t="s">
+      <c r="B77" s="14"/>
+      <c r="C77" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -3130,9 +3130,9 @@
       </c>
     </row>
     <row r="78" spans="2:7">
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="13"/>
       <c r="E78" s="2" t="s">
         <v>190</v>
       </c>
@@ -3144,11 +3144,11 @@
       </c>
     </row>
     <row r="79" spans="2:7">
-      <c r="B79" s="12"/>
-      <c r="C79" s="12" t="s">
+      <c r="B79" s="14"/>
+      <c r="C79" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D79" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E79" s="2" t="s">
@@ -3162,9 +3162,9 @@
       </c>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="13"/>
       <c r="E80" s="2" t="s">
         <v>192</v>
       </c>
@@ -3176,11 +3176,11 @@
       </c>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="12"/>
-      <c r="C81" s="12" t="s">
+      <c r="B81" s="14"/>
+      <c r="C81" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="D81" s="13" t="s">
+      <c r="D81" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E81" s="2" t="s">
@@ -3194,9 +3194,9 @@
       </c>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="13"/>
       <c r="E82" s="2" t="s">
         <v>194</v>
       </c>
@@ -3208,11 +3208,11 @@
       </c>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="12"/>
-      <c r="C83" s="12" t="s">
+      <c r="B83" s="14"/>
+      <c r="C83" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D83" s="13" t="s">
+      <c r="D83" s="12" t="s">
         <v>67</v>
       </c>
       <c r="E83" s="2" t="s">
@@ -3226,9 +3226,9 @@
       </c>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="13"/>
       <c r="E84" s="2" t="s">
         <v>195</v>
       </c>
@@ -3240,11 +3240,11 @@
       </c>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="12"/>
-      <c r="C85" s="12" t="s">
+      <c r="B85" s="14"/>
+      <c r="C85" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D85" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E85" s="2" t="s">
@@ -3256,9 +3256,9 @@
       </c>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="13"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -3281,45 +3281,36 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B7:B22"/>
+    <mergeCell ref="B23:B38"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B39:B54"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C38"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="B71:B86"/>
     <mergeCell ref="C71:C72"/>
@@ -3336,36 +3327,45 @@
     <mergeCell ref="C57:C58"/>
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B54"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B7:B22"/>
-    <mergeCell ref="B23:B38"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="D77:D78"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3388,11 +3388,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733F3413-EE9F-4359-8AAE-13133F084F61}">
   <dimension ref="B1:G87"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="D18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="47.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -3464,10 +3464,10 @@
       </c>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>92</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -3484,8 +3484,8 @@
       </c>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="16"/>
       <c r="E8" s="2" t="s">
         <v>135</v>
@@ -3498,11 +3498,11 @@
       </c>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="12"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>59</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -3516,9 +3516,9 @@
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="2" t="s">
         <v>136</v>
       </c>
@@ -3530,11 +3530,11 @@
       </c>
     </row>
     <row r="11" spans="2:7">
-      <c r="B11" s="12"/>
-      <c r="C11" s="12" t="s">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -3548,9 +3548,9 @@
       </c>
     </row>
     <row r="12" spans="2:7">
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="2" t="s">
         <v>137</v>
       </c>
@@ -3562,11 +3562,11 @@
       </c>
     </row>
     <row r="13" spans="2:7">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -3580,9 +3580,9 @@
       </c>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="2" t="s">
         <v>139</v>
       </c>
@@ -3594,11 +3594,11 @@
       </c>
     </row>
     <row r="15" spans="2:7">
-      <c r="B15" s="12"/>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -3612,9 +3612,9 @@
       </c>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="2" t="s">
         <v>141</v>
       </c>
@@ -3626,11 +3626,11 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="12"/>
-      <c r="C17" s="12" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -3644,9 +3644,9 @@
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="2" t="s">
         <v>143</v>
       </c>
@@ -3658,11 +3658,11 @@
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12" t="s">
+      <c r="B19" s="14"/>
+      <c r="C19" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -3676,9 +3676,9 @@
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="2" t="s">
         <v>145</v>
       </c>
@@ -3690,45 +3690,45 @@
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="12"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>36</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>146</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="G23" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="2" t="s">
         <v>14</v>
       </c>
@@ -3740,11 +3740,11 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>80</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -3758,9 +3758,9 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="2" t="s">
         <v>147</v>
       </c>
@@ -3772,11 +3772,11 @@
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="B27" s="12"/>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -3790,9 +3790,9 @@
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="2" t="s">
         <v>149</v>
       </c>
@@ -3804,11 +3804,11 @@
       </c>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="12"/>
-      <c r="C29" s="12" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -3822,9 +3822,9 @@
       </c>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="2" t="s">
         <v>151</v>
       </c>
@@ -3836,11 +3836,11 @@
       </c>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12" t="s">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -3854,9 +3854,9 @@
       </c>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="13"/>
       <c r="E32" s="2" t="s">
         <v>153</v>
       </c>
@@ -3868,11 +3868,11 @@
       </c>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="12"/>
-      <c r="C33" s="12" t="s">
+      <c r="B33" s="14"/>
+      <c r="C33" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -3886,9 +3886,9 @@
       </c>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="13"/>
       <c r="E34" s="2" t="s">
         <v>155</v>
       </c>
@@ -3900,11 +3900,11 @@
       </c>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="12"/>
-      <c r="C35" s="12" t="s">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -3918,9 +3918,9 @@
       </c>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="14"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="13"/>
       <c r="E36" s="2" t="s">
         <v>157</v>
       </c>
@@ -3932,11 +3932,11 @@
       </c>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="12"/>
-      <c r="C37" s="12" t="s">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>82</v>
       </c>
       <c r="E37" s="2" t="s">
@@ -3950,21 +3950,21 @@
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="14"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="13"/>
       <c r="E38" s="8"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
     </row>
     <row r="39" spans="2:7">
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="D39" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -3978,9 +3978,9 @@
       </c>
     </row>
     <row r="40" spans="2:7">
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="14"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="13"/>
       <c r="E40" s="2" t="s">
         <v>159</v>
       </c>
@@ -3992,11 +3992,11 @@
       </c>
     </row>
     <row r="41" spans="2:7">
-      <c r="B41" s="12"/>
-      <c r="C41" s="12" t="s">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -4010,9 +4010,9 @@
       </c>
     </row>
     <row r="42" spans="2:7">
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="14"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="13"/>
       <c r="E42" s="2" t="s">
         <v>15</v>
       </c>
@@ -4024,11 +4024,11 @@
       </c>
     </row>
     <row r="43" spans="2:7">
-      <c r="B43" s="12"/>
-      <c r="C43" s="12" t="s">
+      <c r="B43" s="14"/>
+      <c r="C43" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="D43" s="12" t="s">
         <v>53</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -4042,9 +4042,9 @@
       </c>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="14"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="13"/>
       <c r="E44" s="2" t="s">
         <v>162</v>
       </c>
@@ -4056,11 +4056,11 @@
       </c>
     </row>
     <row r="45" spans="2:7">
-      <c r="B45" s="12"/>
-      <c r="C45" s="12" t="s">
+      <c r="B45" s="14"/>
+      <c r="C45" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="12" t="s">
         <v>80</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -4074,9 +4074,9 @@
       </c>
     </row>
     <row r="46" spans="2:7">
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="14"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="13"/>
       <c r="E46" s="2" t="s">
         <v>16</v>
       </c>
@@ -4088,11 +4088,11 @@
       </c>
     </row>
     <row r="47" spans="2:7">
-      <c r="B47" s="12"/>
-      <c r="C47" s="12" t="s">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -4106,9 +4106,9 @@
       </c>
     </row>
     <row r="48" spans="2:7">
-      <c r="B48" s="12"/>
-      <c r="C48" s="12"/>
-      <c r="D48" s="14"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="13"/>
       <c r="E48" s="2" t="s">
         <v>165</v>
       </c>
@@ -4120,11 +4120,11 @@
       </c>
     </row>
     <row r="49" spans="2:7">
-      <c r="B49" s="12"/>
-      <c r="C49" s="12" t="s">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D49" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -4138,9 +4138,9 @@
       </c>
     </row>
     <row r="50" spans="2:7">
-      <c r="B50" s="12"/>
-      <c r="C50" s="12"/>
-      <c r="D50" s="14"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="13"/>
       <c r="E50" s="2" t="s">
         <v>167</v>
       </c>
@@ -4152,11 +4152,11 @@
       </c>
     </row>
     <row r="51" spans="2:7">
-      <c r="B51" s="12"/>
-      <c r="C51" s="12" t="s">
+      <c r="B51" s="14"/>
+      <c r="C51" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="D51" s="12" t="s">
         <v>79</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -4170,9 +4170,9 @@
       </c>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="12"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="14"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="13"/>
       <c r="E52" s="2" t="s">
         <v>169</v>
       </c>
@@ -4184,11 +4184,11 @@
       </c>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="12"/>
-      <c r="C53" s="12" t="s">
+      <c r="B53" s="14"/>
+      <c r="C53" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D53" s="12" t="s">
         <v>38</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -4200,21 +4200,21 @@
       </c>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="12"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="14"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="13"/>
       <c r="E54" s="8"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="12" t="s">
+      <c r="B55" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C55" s="12" t="s">
+      <c r="C55" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D55" s="13" t="s">
+      <c r="D55" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -4228,9 +4228,9 @@
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="14"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="13"/>
       <c r="E56" s="2" t="s">
         <v>170</v>
       </c>
@@ -4242,11 +4242,11 @@
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="12"/>
-      <c r="C57" s="12" t="s">
+      <c r="B57" s="14"/>
+      <c r="C57" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D57" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E57" s="10" t="s">
@@ -4260,9 +4260,9 @@
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="14"/>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="13"/>
       <c r="E58" s="2" t="s">
         <v>211</v>
       </c>
@@ -4274,11 +4274,11 @@
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="12"/>
-      <c r="C59" s="12" t="s">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="D59" s="13" t="s">
+      <c r="D59" s="12" t="s">
         <v>205</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -4292,9 +4292,9 @@
       </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="12"/>
-      <c r="C60" s="12"/>
-      <c r="D60" s="14"/>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="13"/>
       <c r="E60" s="2" t="s">
         <v>208</v>
       </c>
@@ -4306,11 +4306,11 @@
       </c>
     </row>
     <row r="61" spans="2:7">
-      <c r="B61" s="12"/>
-      <c r="C61" s="12" t="s">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="D61" s="13" t="s">
+      <c r="D61" s="12" t="s">
         <v>84</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -4324,9 +4324,9 @@
       </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
-      <c r="D62" s="14"/>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="13"/>
       <c r="E62" s="2" t="s">
         <v>176</v>
       </c>
@@ -4338,11 +4338,11 @@
       </c>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="12"/>
-      <c r="C63" s="12" t="s">
+      <c r="B63" s="14"/>
+      <c r="C63" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D63" s="12" t="s">
         <v>206</v>
       </c>
       <c r="E63" s="2" t="s">
@@ -4356,9 +4356,9 @@
       </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="12"/>
-      <c r="C64" s="12"/>
-      <c r="D64" s="14"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="13"/>
       <c r="E64" s="2" t="s">
         <v>177</v>
       </c>
@@ -4370,11 +4370,11 @@
       </c>
     </row>
     <row r="65" spans="2:7">
-      <c r="B65" s="12"/>
-      <c r="C65" s="12" t="s">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D65" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E65" s="2" t="s">
@@ -4388,9 +4388,9 @@
       </c>
     </row>
     <row r="66" spans="2:7">
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="14"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="13"/>
       <c r="E66" s="2" t="s">
         <v>179</v>
       </c>
@@ -4402,11 +4402,11 @@
       </c>
     </row>
     <row r="67" spans="2:7">
-      <c r="B67" s="12"/>
-      <c r="C67" s="12" t="s">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="D67" s="13" t="s">
+      <c r="D67" s="12" t="s">
         <v>54</v>
       </c>
       <c r="E67" s="2" t="s">
@@ -4420,9 +4420,9 @@
       </c>
     </row>
     <row r="68" spans="2:7">
-      <c r="B68" s="12"/>
-      <c r="C68" s="12"/>
-      <c r="D68" s="14"/>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="13"/>
       <c r="E68" s="2" t="s">
         <v>181</v>
       </c>
@@ -4434,11 +4434,11 @@
       </c>
     </row>
     <row r="69" spans="2:7">
-      <c r="B69" s="12"/>
-      <c r="C69" s="12" t="s">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="D69" s="13" t="s">
+      <c r="D69" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E69" s="2" t="s">
@@ -4452,21 +4452,21 @@
       </c>
     </row>
     <row r="70" spans="2:7">
-      <c r="B70" s="12"/>
-      <c r="C70" s="12"/>
-      <c r="D70" s="14"/>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="13"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
     </row>
     <row r="71" spans="2:7">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="12" t="s">
+      <c r="C71" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D71" s="13" t="s">
+      <c r="D71" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -4480,9 +4480,9 @@
       </c>
     </row>
     <row r="72" spans="2:7">
-      <c r="B72" s="12"/>
-      <c r="C72" s="12"/>
-      <c r="D72" s="14"/>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="13"/>
       <c r="E72" s="2" t="s">
         <v>184</v>
       </c>
@@ -4494,11 +4494,11 @@
       </c>
     </row>
     <row r="73" spans="2:7">
-      <c r="B73" s="12"/>
-      <c r="C73" s="12" t="s">
+      <c r="B73" s="14"/>
+      <c r="C73" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D73" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E73" s="2" t="s">
@@ -4512,9 +4512,9 @@
       </c>
     </row>
     <row r="74" spans="2:7">
-      <c r="B74" s="12"/>
-      <c r="C74" s="12"/>
-      <c r="D74" s="14"/>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="13"/>
       <c r="E74" s="2" t="s">
         <v>186</v>
       </c>
@@ -4526,11 +4526,11 @@
       </c>
     </row>
     <row r="75" spans="2:7">
-      <c r="B75" s="12"/>
-      <c r="C75" s="12" t="s">
+      <c r="B75" s="14"/>
+      <c r="C75" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="D75" s="13" t="s">
+      <c r="D75" s="12" t="s">
         <v>33</v>
       </c>
       <c r="E75" s="2" t="s">
@@ -4544,9 +4544,9 @@
       </c>
     </row>
     <row r="76" spans="2:7">
-      <c r="B76" s="12"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="14"/>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="13"/>
       <c r="E76" s="2" t="s">
         <v>188</v>
       </c>
@@ -4558,11 +4558,11 @@
       </c>
     </row>
     <row r="77" spans="2:7">
-      <c r="B77" s="12"/>
-      <c r="C77" s="12" t="s">
+      <c r="B77" s="14"/>
+      <c r="C77" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D77" s="13" t="s">
+      <c r="D77" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -4576,9 +4576,9 @@
       </c>
     </row>
     <row r="78" spans="2:7">
-      <c r="B78" s="12"/>
-      <c r="C78" s="12"/>
-      <c r="D78" s="14"/>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="13"/>
       <c r="E78" s="2" t="s">
         <v>190</v>
       </c>
@@ -4590,11 +4590,11 @@
       </c>
     </row>
     <row r="79" spans="2:7">
-      <c r="B79" s="12"/>
-      <c r="C79" s="12" t="s">
+      <c r="B79" s="14"/>
+      <c r="C79" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="D79" s="13" t="s">
+      <c r="D79" s="12" t="s">
         <v>72</v>
       </c>
       <c r="E79" s="2" t="s">
@@ -4608,9 +4608,9 @@
       </c>
     </row>
     <row r="80" spans="2:7">
-      <c r="B80" s="12"/>
-      <c r="C80" s="12"/>
-      <c r="D80" s="14"/>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="13"/>
       <c r="E80" s="2" t="s">
         <v>192</v>
       </c>
@@ -4622,11 +4622,11 @@
       </c>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="12"/>
-      <c r="C81" s="12" t="s">
+      <c r="B81" s="14"/>
+      <c r="C81" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="D81" s="13" t="s">
+      <c r="D81" s="12" t="s">
         <v>45</v>
       </c>
       <c r="E81" s="2" t="s">
@@ -4640,9 +4640,9 @@
       </c>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="12"/>
-      <c r="C82" s="12"/>
-      <c r="D82" s="14"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="13"/>
       <c r="E82" s="2" t="s">
         <v>194</v>
       </c>
@@ -4654,11 +4654,11 @@
       </c>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="12"/>
-      <c r="C83" s="12" t="s">
+      <c r="B83" s="14"/>
+      <c r="C83" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D83" s="13" t="s">
+      <c r="D83" s="12" t="s">
         <v>67</v>
       </c>
       <c r="E83" s="2" t="s">
@@ -4672,9 +4672,9 @@
       </c>
     </row>
     <row r="84" spans="2:7">
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="14"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="13"/>
       <c r="E84" s="2" t="s">
         <v>195</v>
       </c>
@@ -4686,11 +4686,11 @@
       </c>
     </row>
     <row r="85" spans="2:7">
-      <c r="B85" s="12"/>
-      <c r="C85" s="12" t="s">
+      <c r="B85" s="14"/>
+      <c r="C85" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D85" s="12" t="s">
         <v>63</v>
       </c>
       <c r="E85" s="2" t="s">
@@ -4702,9 +4702,9 @@
       </c>
     </row>
     <row r="86" spans="2:7">
-      <c r="B86" s="12"/>
-      <c r="C86" s="12"/>
-      <c r="D86" s="14"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="13"/>
       <c r="E86" s="2"/>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -4727,6 +4727,75 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="B71:B86"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="B55:B70"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="D65:D66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="B39:B54"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="B23:B38"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="B7:B22"/>
@@ -4743,75 +4812,6 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="B23:B38"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="B39:B54"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="B55:B70"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="B71:B86"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="D81:D82"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>